<commit_message>
Gearing up for R&R
</commit_message>
<xml_diff>
--- a/1 Stim/Recall and Recog/Mediated Stim_All.xlsx
+++ b/1 Stim/Recall and Recog/Mediated Stim_All.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\OneDrive\Documents\GitHub\Mediated-Reactivity\1 Stim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\OneDrive\Documents\GitHub\Mediated-Reactivity\1 Stim\Recall and Recog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292B32C1-315C-4864-A719-F5F05023EC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16340E5E-E3F8-42A3-813B-6E071466C826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{4E90AFB4-3589-4698-9593-B034AD7F1DE8}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11380" windowHeight="13370" activeTab="1" xr2:uid="{4E90AFB4-3589-4698-9593-B034AD7F1DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mediated Pairs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="231">
   <si>
     <t>Cue</t>
   </si>
@@ -636,6 +637,99 @@
   </si>
   <si>
     <t>Children</t>
+  </si>
+  <si>
+    <t>Mediator</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Peace</t>
+  </si>
+  <si>
+    <t>Smooth</t>
+  </si>
+  <si>
+    <t>Maple</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Night</t>
+  </si>
+  <si>
+    <t>Brush</t>
+  </si>
+  <si>
+    <t>Soft</t>
+  </si>
+  <si>
+    <t>FAS</t>
+  </si>
+  <si>
+    <t>Stripe</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Nose</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>Grass</t>
   </si>
 </sst>
 </file>
@@ -1013,9 +1107,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62822242-3420-4550-A069-F6E0B72359D0}">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V62" sqref="V62"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4737,4 +4831,741 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4E212F-371B-48C6-A650-8C09BD603053}">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L2">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="N2" t="s">
+        <v>229</v>
+      </c>
+      <c r="O2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" t="s">
+        <v>218</v>
+      </c>
+      <c r="L3">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>218</v>
+      </c>
+      <c r="O3" t="s">
+        <v>96</v>
+      </c>
+      <c r="P3">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="E4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" t="s">
+        <v>219</v>
+      </c>
+      <c r="L4">
+        <v>0.185</v>
+      </c>
+      <c r="N4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5">
+        <v>0.192</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L5">
+        <v>0.128</v>
+      </c>
+      <c r="N5" t="s">
+        <v>220</v>
+      </c>
+      <c r="O5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6">
+        <v>0.06</v>
+      </c>
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" t="s">
+        <v>221</v>
+      </c>
+      <c r="L6">
+        <v>0.121</v>
+      </c>
+      <c r="N6" t="s">
+        <v>221</v>
+      </c>
+      <c r="O6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P6">
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="J7" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" t="s">
+        <v>222</v>
+      </c>
+      <c r="L7">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="N7" t="s">
+        <v>222</v>
+      </c>
+      <c r="O7" t="s">
+        <v>104</v>
+      </c>
+      <c r="P7">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8">
+        <v>0.252</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>0.06</v>
+      </c>
+      <c r="J8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>132</v>
+      </c>
+      <c r="O8" t="s">
+        <v>106</v>
+      </c>
+      <c r="P8">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>0.02</v>
+      </c>
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9" t="s">
+        <v>223</v>
+      </c>
+      <c r="L9">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="N9" t="s">
+        <v>223</v>
+      </c>
+      <c r="O9" t="s">
+        <v>108</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" t="s">
+        <v>230</v>
+      </c>
+      <c r="L10">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>230</v>
+      </c>
+      <c r="O10" t="s">
+        <v>110</v>
+      </c>
+      <c r="P10">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11">
+        <v>0.218</v>
+      </c>
+      <c r="E11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" t="s">
+        <v>228</v>
+      </c>
+      <c r="L11">
+        <v>2.3E-2</v>
+      </c>
+      <c r="N11" t="s">
+        <v>228</v>
+      </c>
+      <c r="O11" t="s">
+        <v>112</v>
+      </c>
+      <c r="P11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12">
+        <v>0.109</v>
+      </c>
+      <c r="E12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" t="s">
+        <v>227</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>227</v>
+      </c>
+      <c r="O12" t="s">
+        <v>114</v>
+      </c>
+      <c r="P12">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="J13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" t="s">
+        <v>226</v>
+      </c>
+      <c r="L13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>226</v>
+      </c>
+      <c r="O13" t="s">
+        <v>116</v>
+      </c>
+      <c r="P13">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C14">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="E14" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14">
+        <v>0.192</v>
+      </c>
+      <c r="J14" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" t="s">
+        <v>225</v>
+      </c>
+      <c r="L14">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="N14" t="s">
+        <v>225</v>
+      </c>
+      <c r="O14" t="s">
+        <v>118</v>
+      </c>
+      <c r="P14">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15">
+        <v>0.123</v>
+      </c>
+      <c r="E15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15">
+        <v>0.44</v>
+      </c>
+      <c r="J15" t="s">
+        <v>119</v>
+      </c>
+      <c r="K15" t="s">
+        <v>224</v>
+      </c>
+      <c r="L15">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="N15" t="s">
+        <v>224</v>
+      </c>
+      <c r="O15" t="s">
+        <v>120</v>
+      </c>
+      <c r="P15">
+        <v>0.13900000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="E16" t="s">
+        <v>213</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L16">
+        <v>0.161</v>
+      </c>
+      <c r="N16" t="s">
+        <v>124</v>
+      </c>
+      <c r="O16" t="s">
+        <v>122</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18">
+        <f>AVERAGE(C2:C16)</f>
+        <v>0.29086666666666666</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18">
+        <f>AVERAGE(G2:G16)</f>
+        <v>0.112</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L18">
+        <f>AVERAGE(L2:L16)</f>
+        <v>0.16899999999999998</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P18">
+        <f>AVERAGE(P2:P16)</f>
+        <v>6.660000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19">
+        <f>STDEV(C2:C16)</f>
+        <v>0.23784114346304666</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19">
+        <f>STDEV(G2:G16)</f>
+        <v>0.13012576334344514</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L19">
+        <f>STDEV(L2:L16)</f>
+        <v>0.15336976792799067</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P19">
+        <f>STDEV(P2:P16)</f>
+        <v>6.3738080118111939E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="B21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G21">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="L21">
+        <v>0.622</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="P21">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>